<commit_message>
add import excel function
</commit_message>
<xml_diff>
--- a/server/resource/excel/ExcelImport.xlsx
+++ b/server/resource/excel/ExcelImport.xlsx
@@ -1,79 +1,88 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA2E71E-CEDE-4383-8B66-A95FE11F0809}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="3696" yWindow="2700" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>路由Name</t>
-  </si>
-  <si>
-    <t>路由Path</t>
-  </si>
-  <si>
-    <t>是否隐藏</t>
-  </si>
-  <si>
-    <t>父节点</t>
-  </si>
-  <si>
-    <t>文件名称</t>
-  </si>
-  <si>
-    <t>https://www.gin-vue-admin.com</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>排序</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+  <si>
+    <t>系统名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>内网ip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>内网ip端口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否测试环境（是/否）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>产品经理（产品线-负责人）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>域名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外网ip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外网ip端口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -96,9 +105,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -117,7 +125,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -369,99 +377,417 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="24.875" customWidth="1"/>
+    <col min="4" max="4" width="18.625" customWidth="1"/>
+    <col min="8" max="8" width="16.625" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8">
         <v>7</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10">
         <v>9</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>